<commit_message>
here is the latest gantt chart
</commit_message>
<xml_diff>
--- a/gantt_chart.xlsx
+++ b/gantt_chart.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>Task</t>
   </si>
@@ -51,9 +51,6 @@
     <t>ESL Project</t>
   </si>
   <si>
-    <t>Project Proposal (Introduction)</t>
-  </si>
-  <si>
     <t>Make Rationale of the Study</t>
   </si>
   <si>
@@ -103,6 +100,18 @@
   </si>
   <si>
     <t>Complete</t>
+  </si>
+  <si>
+    <t>The Problem</t>
+  </si>
+  <si>
+    <t>Statement of the Problem</t>
+  </si>
+  <si>
+    <t>Significance of the Study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project Proposal </t>
   </si>
 </sst>
 </file>
@@ -170,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -186,23 +195,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -214,13 +214,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -266,6 +259,18 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -317,11 +322,11 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$10:$A$21</c:f>
+              <c:f>Sheet1!$A$10:$A$24</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>Project Proposal (Introduction)</c:v>
+                  <c:v>Project Proposal </c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Research About The Topic</c:v>
@@ -354,6 +359,15 @@
                   <c:v>Treatment of Data</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>The Problem</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Statement of the Problem</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Significance of the Study</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>Checking </c:v>
                 </c:pt>
               </c:strCache>
@@ -361,10 +375,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$10:$B$20</c:f>
+              <c:f>Sheet1!$B$10:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>42332</c:v>
                 </c:pt>
@@ -377,6 +391,9 @@
                 <c:pt idx="3">
                   <c:v>42333</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>42334</c:v>
+                </c:pt>
                 <c:pt idx="5">
                   <c:v>42334</c:v>
                 </c:pt>
@@ -394,6 +411,18 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>42334</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42335</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42335</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42335</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42336</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -416,11 +445,11 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$10:$A$21</c:f>
+              <c:f>Sheet1!$A$10:$A$24</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>Project Proposal (Introduction)</c:v>
+                  <c:v>Project Proposal </c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Research About The Topic</c:v>
@@ -453,6 +482,15 @@
                   <c:v>Treatment of Data</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>The Problem</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Statement of the Problem</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Significance of the Study</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>Checking </c:v>
                 </c:pt>
               </c:strCache>
@@ -460,12 +498,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$10:$D$21</c:f>
+              <c:f>Sheet1!$D$10:$D$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -477,7 +515,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
@@ -498,6 +536,15 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -514,11 +561,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="69023232"/>
-        <c:axId val="69024768"/>
+        <c:axId val="89187840"/>
+        <c:axId val="89189376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="69023232"/>
+        <c:axId val="89187840"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -528,7 +575,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69024768"/>
+        <c:crossAx val="89189376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -536,7 +583,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69024768"/>
+        <c:axId val="89189376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42368"/>
@@ -549,7 +596,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69023232"/>
+        <c:crossAx val="89187840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="7"/>
@@ -580,8 +627,8 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>156882</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -590,8 +637,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7400925" y="1323975"/>
-          <a:ext cx="1628775" cy="1571625"/>
+          <a:off x="9667315" y="1323975"/>
+          <a:ext cx="1628214" cy="1499907"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -883,15 +930,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:colOff>246528</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:colOff>342899</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>33618</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -900,8 +947,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9867900" y="2390775"/>
-          <a:ext cx="114300" cy="104775"/>
+          <a:off x="9894793" y="2390775"/>
+          <a:ext cx="96371" cy="119343"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1022,14 +1069,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>109777</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>109775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>67357</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>185977</xdr:rowOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1048,6 +1095,112 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>235323</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>112059</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Diamond 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9883588" y="2588559"/>
+          <a:ext cx="145677" cy="168088"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>504265</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="401777" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10152530" y="2521324"/>
+          <a:ext cx="401777" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>End</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1055,12 +1208,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.22714</cdr:x>
-      <cdr:y>0.10762</cdr:y>
+      <cdr:x>0.25276</cdr:x>
+      <cdr:y>0.09155</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.24309</cdr:x>
-      <cdr:y>0.21734</cdr:y>
+      <cdr:x>0.26315</cdr:x>
+      <cdr:y>0.16296</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -1069,8 +1222,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="3680614" y="295223"/>
-          <a:ext cx="258451" cy="300984"/>
+          <a:off x="4095746" y="303880"/>
+          <a:ext cx="168213" cy="237029"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="diamond">
           <a:avLst/>
@@ -1103,12 +1256,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.29692</cdr:x>
-      <cdr:y>0.2433</cdr:y>
+      <cdr:x>0.31698</cdr:x>
+      <cdr:y>0.21967</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.40069</cdr:x>
-      <cdr:y>0.4814</cdr:y>
+      <cdr:x>0.42075</cdr:x>
+      <cdr:y>0.45777</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -1117,8 +1270,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="4811223" y="667432"/>
-          <a:ext cx="1681472" cy="653142"/>
+          <a:off x="5136212" y="729127"/>
+          <a:ext cx="1681471" cy="790306"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -1154,7 +1307,7 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>(November 28, 2015 - Saturday )</a:t>
+            <a:t>(November 29, 2015 - Saturday )</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -1163,12 +1316,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.24447</cdr:x>
-      <cdr:y>0.16015</cdr:y>
+      <cdr:x>0.26453</cdr:x>
+      <cdr:y>0.12549</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.29634</cdr:x>
-      <cdr:y>0.31538</cdr:y>
+      <cdr:x>0.3164</cdr:x>
+      <cdr:y>0.28072</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
@@ -1177,8 +1330,8 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="3961426" y="439311"/>
-          <a:ext cx="840492" cy="425827"/>
+          <a:off x="4286320" y="416535"/>
+          <a:ext cx="840492" cy="515243"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="bentConnector3">
           <a:avLst/>
@@ -1203,25 +1356,212 @@
       </cdr:style>
     </cdr:cxnSp>
   </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.21023</cdr:x>
+      <cdr:y>0.32817</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.21853</cdr:x>
+      <cdr:y>0.37881</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="Diamond 3"/>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3406589" y="1089255"/>
+          <a:ext cx="134471" cy="168088"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.23342</cdr:x>
+      <cdr:y>0.73778</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.24172</cdr:x>
+      <cdr:y>0.78842</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="7" name="Diamond 6"/>
+        <cdr:cNvSpPr/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3782359" y="2448859"/>
+          <a:ext cx="134471" cy="168088"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
 </c:userShapes>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A8:H21" totalsRowShown="0">
-  <autoFilter ref="A8:H21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A8:H24" totalsRowShown="0">
+  <autoFilter ref="A8:H24"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Task"/>
-    <tableColumn id="2" name="Start Date" dataDxfId="3"/>
-    <tableColumn id="3" name="End Date" dataDxfId="2"/>
-    <tableColumn id="4" name="Duration" dataDxfId="1">
+    <tableColumn id="2" name="Start Date" dataDxfId="11"/>
+    <tableColumn id="3" name="End Date" dataDxfId="10"/>
+    <tableColumn id="4" name="Duration" dataDxfId="9">
       <calculatedColumnFormula>Table2[[#This Row],[End Date]]-Table2[[#This Row],[Start Date]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="Assigned To"/>
     <tableColumn id="6" name="Status"/>
-    <tableColumn id="9" name="% Complete" dataDxfId="0"/>
+    <tableColumn id="9" name="% Complete" dataDxfId="8"/>
     <tableColumn id="7" name="Comments"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1512,10 +1852,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:K21"/>
+  <dimension ref="A5:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1576,24 +1916,24 @@
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>11</v>
+      <c r="A10" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="B10" s="5">
         <v>42332</v>
       </c>
       <c r="C10" s="5">
-        <v>42336</v>
+        <v>42337</v>
       </c>
       <c r="D10">
         <f>Table2[[#This Row],[End Date]]-Table2[[#This Row],[Start Date]]</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10" s="1">
         <v>1</v>
@@ -1601,7 +1941,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="5">
         <v>42332</v>
@@ -1617,7 +1957,7 @@
         <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G11" s="1">
         <v>1</v>
@@ -1625,7 +1965,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="5">
         <v>42333</v>
@@ -1641,7 +1981,7 @@
         <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G12" s="1">
         <v>1</v>
@@ -1649,7 +1989,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="5">
         <v>42333</v>
@@ -1662,10 +2002,10 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="F13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G13" s="1">
         <v>1</v>
@@ -1673,19 +2013,23 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="B14" s="5">
+        <v>42334</v>
+      </c>
+      <c r="C14" s="5">
+        <v>42335</v>
+      </c>
       <c r="D14" s="2">
         <f>Table2[[#This Row],[End Date]]-Table2[[#This Row],[Start Date]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" t="s">
         <v>9</v>
       </c>
       <c r="F14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G14" s="1">
         <v>0</v>
@@ -1693,7 +2037,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="5">
         <v>42334</v>
@@ -1706,10 +2050,10 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G15" s="1">
         <v>0</v>
@@ -1717,7 +2061,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="5">
         <v>42334</v>
@@ -1730,10 +2074,10 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G16" s="1">
         <v>0</v>
@@ -1741,7 +2085,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="5">
         <v>42334</v>
@@ -1754,10 +2098,10 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G17" s="1">
         <v>0</v>
@@ -1765,7 +2109,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="5">
         <v>42334</v>
@@ -1781,7 +2125,7 @@
         <v>8</v>
       </c>
       <c r="F18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G18" s="1">
         <v>0</v>
@@ -1789,7 +2133,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="5">
         <v>42334</v>
@@ -1802,10 +2146,10 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G19" s="1">
         <v>0</v>
@@ -1813,7 +2157,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="5">
         <v>42334</v>
@@ -1826,10 +2170,10 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G20" s="1">
         <v>0</v>
@@ -1837,77 +2181,132 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B21" s="5">
         <v>42335</v>
       </c>
       <c r="C21" s="5">
-        <v>42335</v>
+        <v>42336</v>
       </c>
       <c r="D21" s="2">
         <f>Table2[[#This Row],[End Date]]-Table2[[#This Row],[Start Date]]</f>
+        <v>1</v>
+      </c>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="5">
+        <v>42335</v>
+      </c>
+      <c r="C22" s="5">
+        <v>42336</v>
+      </c>
+      <c r="D22" s="2">
+        <f>Table2[[#This Row],[End Date]]-Table2[[#This Row],[Start Date]]</f>
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="5">
+        <v>42335</v>
+      </c>
+      <c r="C23" s="5">
+        <v>42336</v>
+      </c>
+      <c r="D23" s="2">
+        <f>Table2[[#This Row],[End Date]]-Table2[[#This Row],[Start Date]]</f>
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="5">
+        <v>42336</v>
+      </c>
+      <c r="C24" s="5">
+        <v>42336</v>
+      </c>
+      <c r="D24" s="2">
+        <f>Table2[[#This Row],[End Date]]-Table2[[#This Row],[Start Date]]</f>
         <v>0</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E24" t="s">
         <v>9</v>
       </c>
-      <c r="F21" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="1">
+      <c r="F24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E9:E21">
-    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="Tibon">
+  <conditionalFormatting sqref="E9:E24">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Tibon">
       <formula>NOT(ISERROR(SEARCH("Tibon",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="Alipar">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Alipar">
       <formula>NOT(ISERROR(SEARCH("Alipar",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="Canono">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="Canono">
       <formula>NOT(ISERROR(SEARCH("Canono",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="Banico">
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="Banico">
       <formula>NOT(ISERROR(SEARCH("Banico",E9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="Caballero">
+    <cfRule type="containsText" dxfId="3" priority="9" operator="containsText" text="Caballero">
       <formula>NOT(ISERROR(SEARCH("Caballero",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E9 E16:E20">
-    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="All">
+  <conditionalFormatting sqref="E9:E23">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="All">
       <formula>NOT(ISERROR(SEARCH("All",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10:E15">
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="All">
-      <formula>NOT(ISERROR(SEARCH("All",E10)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E10:E20">
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="Caballero">
+  <conditionalFormatting sqref="E10:E23">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Caballero">
       <formula>NOT(ISERROR(SEARCH("Caballero",E10)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="All">
-      <formula>NOT(ISERROR(SEARCH("All",E21)))</formula>
+  <conditionalFormatting sqref="E24">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="All">
+      <formula>NOT(ISERROR(SEARCH("All",E24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E8 E22:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E8 E25:E1048576">
       <formula1>"Caballero, Canono, Banico, Alipar, Tibon"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9:F21">
-      <formula1>"Complete, Not Complete"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9">
       <formula1>"All,Caballero, Canono, Banico, Alipar, Tibon"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10:E20 E21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F9:F24">
+      <formula1>"Complete, Not Complete"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10:E24">
       <formula1>"All, Caballero, Canono, Banico, Alipar, Tibon"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>